<commit_message>
Connection to Database works fine, write values too. TODO: read values and calculate changes
</commit_message>
<xml_diff>
--- a/Values.xlsx
+++ b/Values.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://szybbs-my.sharepoint.com/personal/martin_stadler_sz-ybbs_ac_at/Documents/In/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marts\PycharmProjects\CCA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="40" documentId="8_{DFE14262-F6B7-47E6-A41A-9ECEEF964626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{76225AE0-ADBC-4E08-86EA-7FAA8057313D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{077A72E8-17A5-4550-8433-2706B8B62966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BC1C4270-E68A-4082-A108-6445BE0BACE0}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="75">
   <si>
     <t>Cryptodata</t>
   </si>
@@ -256,6 +256,9 @@
   </si>
   <si>
     <t>social_contributors_change_rel</t>
+  </si>
+  <si>
+    <t>Updated 31.07.2021</t>
   </si>
 </sst>
 </file>
@@ -629,10 +632,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3817D932-0685-414B-AD91-C86B85F512D9}">
-  <dimension ref="A2:U39"/>
+  <dimension ref="A2:U48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -960,6 +963,11 @@
       </c>
       <c r="C39" s="4"/>
     </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>74</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>